<commit_message>
Updated list of functions
</commit_message>
<xml_diff>
--- a/list_of_functions.xlsx
+++ b/list_of_functions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeann\OneDrive\Documents\GitHub\classe-time-tabling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeann\OneDrive\Documents\GitHub\course-time-tabling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FCCCBB-EECA-414E-82E5-E1EFF1F05A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD26EF55-2071-43D0-9A0C-06B9999410D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="512" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>baseSelectorCourses</t>
   </si>
@@ -420,13 +420,74 @@
   </si>
   <si>
     <t>Returns all the students' Ids</t>
+  </si>
+  <si>
+    <t>HappinessList</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(n: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Creates a list which we will use to give the happiness values</t>
+  </si>
+  <si>
+    <t>HappinessMeter</t>
+  </si>
+  <si>
+    <t>Calculates the total happiness for a given solution in dictionary form (dictionary with courses as the keys)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(solution: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dict</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,6 +506,12 @@
     <font>
       <sz val="11"/>
       <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -511,8 +578,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4505AAA7-6B20-4BA8-B005-B4140B0B8AB5}" name="Tableau1" displayName="Tableau1" ref="A1:D16" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D16" xr:uid="{4505AAA7-6B20-4BA8-B005-B4140B0B8AB5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4505AAA7-6B20-4BA8-B005-B4140B0B8AB5}" name="Tableau1" displayName="Tableau1" ref="A1:D18" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:D18" xr:uid="{4505AAA7-6B20-4BA8-B005-B4140B0B8AB5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{766DC959-4B2F-41C7-8890-BF43DE00A27F}" name="Name"/>
     <tableColumn id="2" xr3:uid="{9ED1F58F-0C00-462E-9F7C-5D69C0DD78DB}" name="Input"/>
@@ -786,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,7 +864,7 @@
     <col min="1" max="1" width="28.5546875" customWidth="1"/>
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
     <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="69.5546875" customWidth="1"/>
+    <col min="4" max="4" width="88" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1022,6 +1089,34 @@
       </c>
       <c r="D16" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>